<commit_message>
onglet 2858 et barème ancienneté
</commit_message>
<xml_diff>
--- a/src/VehicleTaxReport/VehicleTaxReport.xlsx
+++ b/src/VehicleTaxReport/VehicleTaxReport.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wanamicsfr-my.sharepoint.com/personal/cwatrelot_wanamics_fr/Documents/AL/WanaFrance/src/VehicleTaxReport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:1_{771DC25A-BB0C-4C18-8158-9411850FC94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C97898-A2F1-433C-B055-CA58FF854071}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="13_ncr:1_{771DC25A-BB0C-4C18-8158-9411850FC94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D0E6F64-13B7-42AD-B822-620072D65F10}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="-16320" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="-16320" windowWidth="29040" windowHeight="16440" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="7" state="hidden" r:id="rId1"/>
     <sheet name="Report Metadata" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Barême CO2" sheetId="6" state="hidden" r:id="rId3"/>
-    <sheet name="2857-FC-SD" sheetId="4" r:id="rId4"/>
-    <sheet name="2858-FC-SD" sheetId="5" r:id="rId5"/>
+    <sheet name="Coef. pondérateur" sheetId="9" state="hidden" r:id="rId4"/>
+    <sheet name="Barème ancienneté" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="2857-FC-SD" sheetId="4" r:id="rId6"/>
+    <sheet name="2858-FC-SD" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="95">
   <si>
     <t>No</t>
   </si>
@@ -336,6 +338,27 @@
   <si>
     <t>TaxEndingDate</t>
   </si>
+  <si>
+    <t>Tarif gazole et assimilé</t>
+  </si>
+  <si>
+    <t>Tarif autre</t>
+  </si>
+  <si>
+    <t>Nb. Km remboursés</t>
+  </si>
+  <si>
+    <t>% taxe à reverser</t>
+  </si>
+  <si>
+    <t>Gazole</t>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t>Année 1ère immat. (à partir de)</t>
+  </si>
 </sst>
 </file>
 
@@ -344,9 +367,16 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -557,179 +587,183 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="18" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -2053,7 +2087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897751AA-AEC8-42DA-90B9-E3EF87E570E1}">
   <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
@@ -4078,13 +4112,154 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB357A07-4FA6-4D6C-A605-BA47CF4CA816}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>15001</v>
+      </c>
+      <c r="B3" s="59">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>25001</v>
+      </c>
+      <c r="B4" s="59">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>35001</v>
+      </c>
+      <c r="B5" s="59">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>45001</v>
+      </c>
+      <c r="B6" s="59">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CCDB01-AF5C-4F21-AA21-891EBF3E0C4F}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="52" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>600</v>
+      </c>
+      <c r="C2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2001</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="62">
+        <v>2006</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2011</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2015</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30845292-5431-4A4E-B0C6-18BCB618A099}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+    <sheetView showZeros="0" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4393,12 +4568,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3965F3-D149-4451-A68D-3862368B16E1}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4542,6 +4717,30 @@
         <v>37</v>
       </c>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5" s="60">
+        <v>40544</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="2">
+        <f>IF(D5="Gazole",_xlfn.XLOOKUP(YEAR(B5),'Barème ancienneté'!A:A,'Barème ancienneté'!B:B,0,-1),_xlfn.XLOOKUP(YEAR(B5),'Barème ancienneté'!A:A,'Barème ancienneté'!C:C,0,-1))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B6" s="60">
+        <v>43831</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="2">
+        <f>IF(D6="Gazole",_xlfn.XLOOKUP(YEAR(B6),'Barème ancienneté'!A:A,'Barème ancienneté'!B:B,0,-1),_xlfn.XLOOKUP(YEAR(B6),'Barème ancienneté'!A:A,'Barème ancienneté'!C:C,0,-1))</f>
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:O1"/>

</xml_diff>